<commit_message>
Update for release mines - January 30
</commit_message>
<xml_diff>
--- a/2130 Coal Mine, China, M1809.xlsx
+++ b/2130 Coal Mine, China, M1809.xlsx
@@ -432,7 +432,7 @@
     <row r="2" ht="15.75" customHeight="1" s="12">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Version: mines - January 30 (built on January 30 2026 16.19.47 EST)</t>
+          <t>Version: mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
         </is>
       </c>
       <c r="H2" s="2" t="n"/>
@@ -538,7 +538,7 @@
     <row r="6" ht="15.75" customHeight="1" s="12">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'mines - January 30 (built on January 30 2026 16.19.47 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
+          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'mines - January 30 (built on February 02 2026 12.49.33 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
         </is>
       </c>
       <c r="H6" s="2" t="n"/>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on January 30 2026 16.19.47 EST)</t>
+          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
         </is>
       </c>
       <c r="T2" s="0" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on January 30 2026 16.19.47 EST)</t>
+          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
         </is>
       </c>
       <c r="T3" s="0" t="inlineStr">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on January 30 2026 16.19.47 EST)</t>
+          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on January 30 2026 16.19.47 EST)</t>
+          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">

</xml_diff>

<commit_message>
Update for release mines - version 1.0.0 (Feb 3 2026)
</commit_message>
<xml_diff>
--- a/2130 Coal Mine, China, M1809.xlsx
+++ b/2130 Coal Mine, China, M1809.xlsx
@@ -432,7 +432,7 @@
     <row r="2" ht="15.75" customHeight="1" s="12">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Version: mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
+          <t>Version: mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
         </is>
       </c>
       <c r="H2" s="2" t="n"/>
@@ -538,7 +538,7 @@
     <row r="6" ht="15.75" customHeight="1" s="12">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'mines - January 30 (built on February 02 2026 12.49.33 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
+          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
         </is>
       </c>
       <c r="H6" s="2" t="n"/>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
+          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
         </is>
       </c>
       <c r="T2" s="0" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
+          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
         </is>
       </c>
       <c r="T3" s="0" t="inlineStr">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
+          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>mines - January 30 (built on February 02 2026 12.49.33 EST)</t>
+          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">

</xml_diff>

<commit_message>
Update for release Coal Mine Boundaries and Methane Sources - version 1.0.0
</commit_message>
<xml_diff>
--- a/2130 Coal Mine, China, M1809.xlsx
+++ b/2130 Coal Mine, China, M1809.xlsx
@@ -432,7 +432,7 @@
     <row r="2" ht="15.75" customHeight="1" s="12">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Version: mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
+          <t>Version: Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)</t>
         </is>
       </c>
       <c r="H2" s="2" t="n"/>
@@ -538,7 +538,7 @@
     <row r="6" ht="15.75" customHeight="1" s="12">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
+          <t>Recommended Citation:  "Global Energy Monitor, Coal mine boundaries and methane sources for 2130 Coal Mine, China, M1809, version 'Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)'. (See the CC license for attribution requirements if sharing or adapting the data set.)</t>
         </is>
       </c>
       <c r="H6" s="2" t="n"/>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
+          <t>Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)</t>
         </is>
       </c>
       <c r="T2" s="0" t="inlineStr">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
+          <t>Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)</t>
         </is>
       </c>
       <c r="T3" s="0" t="inlineStr">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
+          <t>Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
@@ -2562,7 +2562,7 @@
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>mines - version 1.0.0 (Feb 3 2026) (built on February 03 2026 10.14.00 EST)</t>
+          <t>Coal Mine Boundaries and Methane Sources - version 1.0.0 (built on February 03 2026 17.29.55 EST)</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">

</xml_diff>